<commit_message>
Added final project 3 codes with 9 test cases
</commit_message>
<xml_diff>
--- a/TestDatas/credentials.xlsx
+++ b/TestDatas/credentials.xlsx
@@ -499,11 +499,11 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45851</v>
+        <v>45852</v>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>22:18:58</t>
+          <t>01:35:30</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -534,11 +534,11 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45851</v>
+        <v>45852</v>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>22:19:05</t>
+          <t>01:35:37</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -569,11 +569,11 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45851</v>
+        <v>45852</v>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>22:19:06</t>
+          <t>01:35:37</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
@@ -604,11 +604,11 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45851</v>
+        <v>45852</v>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>22:19:13</t>
+          <t>01:35:44</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">

</xml_diff>